<commit_message>
adiciona ranking de mitica
</commit_message>
<xml_diff>
--- a/classes.xlsx
+++ b/classes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,11 @@
           <t>Melhores DPS em Raids</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Melhores DPS em Míticas</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -446,6 +451,11 @@
           <t>Havoc Demon Hunter (A Tier)</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Shadow Priest (S Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -453,6 +463,11 @@
           <t>Augmentation Evoker (A Tier)</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Fire Mage (A Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -460,6 +475,11 @@
           <t>Enhancement Shaman (A Tier)</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Augmentation Evoker(A Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -467,6 +487,11 @@
           <t>Beast Mastery Hunter (A Tier)</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Frost Mage (A Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -474,6 +499,11 @@
           <t>Assassination Rogue (A Tier)</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Outlaw Rogue (A Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -481,6 +511,11 @@
           <t>Subtlety Rogue (A Tier)</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Destruction Warlock (A Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -488,6 +523,11 @@
           <t>Feral Druid (A Tier)</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Devastation Evoker (B Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -495,6 +535,11 @@
           <t>Arcane Mage (B Tier)</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Balance Druid (B Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -502,6 +547,11 @@
           <t>Fire Mage (B Tier)</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Demonology Warlock (B Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -509,6 +559,11 @@
           <t>Balance Druid (B Tier)</t>
         </is>
       </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Arms Warrior (B Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -516,6 +571,11 @@
           <t>Outlaw Rogue (B Tier)</t>
         </is>
       </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Windwalker Monk (B Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -523,6 +583,11 @@
           <t>Fury Warrior (B Tier)</t>
         </is>
       </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Beast Mastery Hunter (B Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -530,6 +595,11 @@
           <t>Elemental Shaman (B Tier)</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Demonology Warlock (B Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -537,6 +607,11 @@
           <t>Survival Hunter (B Tier)</t>
         </is>
       </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Subtlety Rogue (B Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -544,6 +619,11 @@
           <t>Demonology Warlock (B Tier)</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Retribution Paladin (B Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -551,6 +631,11 @@
           <t>Frost Death Knight (B Tier)</t>
         </is>
       </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Assassination Rogue (C Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -558,6 +643,11 @@
           <t>Frost Mage (B Tier)</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Marksmanship Hunter (C Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -565,6 +655,11 @@
           <t>Devastation Evoker (C Tier)</t>
         </is>
       </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Fury Warrior (C Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -572,6 +667,11 @@
           <t>Arms Warrior (C Tier)</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Unholy Death Knight (C Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -579,6 +679,11 @@
           <t>Shadow Priest (C Tier)</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Elemental Shaman (C Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -586,6 +691,11 @@
           <t>Retribution Paladin (C Tier)</t>
         </is>
       </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Frost Death Knight (C Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -593,6 +703,11 @@
           <t>Destruction Warlock (C Tier)</t>
         </is>
       </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Arcane Mage (C Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -600,6 +715,11 @@
           <t>Unholy Death Knight (C Tier)</t>
         </is>
       </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Assassination Rogue (C Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -607,6 +727,11 @@
           <t>Marksmanship Hunter (D Tier)</t>
         </is>
       </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Enhancement Shaman (C Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -614,11 +739,37 @@
           <t>Affliction Warlock (D Tier)</t>
         </is>
       </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Havoc Demon Hunter (C Tier)</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
           <t>Windwalker Monk (D Tier)</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Affliction Warlock (D Tier)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Feral Druid (D Tier)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Survival Hunter (D Tier)</t>
         </is>
       </c>
     </row>

</xml_diff>